<commit_message>
6 times faster Student distribution
By eliminating many conversions, the IL will be also 752 bytes (47%) smaller
</commit_message>
<xml_diff>
--- a/ILSIze.xlsx
+++ b/ILSIze.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5C7A7C-FA8C-454F-B3FB-C31CA50635BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7284AE1E-FD30-B542-A046-A6639A12F59E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35280" yWindow="-860" windowWidth="25440" windowHeight="14400" activeTab="3" xr2:uid="{E50D0282-9BF7-F541-B69F-D7AC36D41BED}"/>
+    <workbookView xWindow="35280" yWindow="-860" windowWidth="25440" windowHeight="14400" activeTab="4" xr2:uid="{E50D0282-9BF7-F541-B69F-D7AC36D41BED}"/>
   </bookViews>
   <sheets>
     <sheet name="Chemistry.cs" sheetId="1" r:id="rId1"/>
     <sheet name="EnzymeKinematic" sheetId="2" r:id="rId2"/>
     <sheet name="void OutputEnzymeKinematic" sheetId="3" r:id="rId3"/>
     <sheet name="LinearRegression.cs" sheetId="4" r:id="rId4"/>
+    <sheet name="Student" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Méthode</t>
   </si>
@@ -183,6 +184,57 @@
   </si>
   <si>
     <t>Itération 5</t>
+  </si>
+  <si>
+    <t>Ancienne</t>
+  </si>
+  <si>
+    <t>Nouvelle</t>
+  </si>
+  <si>
+    <t>AddGammaFactors</t>
+  </si>
+  <si>
+    <t>AddGammaIntegers</t>
+  </si>
+  <si>
+    <t>AddGammaHalves</t>
+  </si>
+  <si>
+    <t>BigProduct</t>
+  </si>
+  <si>
+    <t>(Fast)GammaRatio</t>
+  </si>
+  <si>
+    <t>HugeProduct</t>
+  </si>
+  <si>
+    <t>MultiplyByFractions</t>
+  </si>
+  <si>
+    <t>(Old)Student</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>ProductOfIntegers</t>
+  </si>
+  <si>
+    <t>Regroup</t>
+  </si>
+  <si>
+    <t>RemoveDividableFactors</t>
+  </si>
+  <si>
+    <t>RemoveIdenticalFactors</t>
+  </si>
+  <si>
+    <t>SplitDividableBy</t>
+  </si>
+  <si>
+    <t>TryMultiply</t>
   </si>
 </sst>
 </file>
@@ -242,13 +294,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,16 +655,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1154,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14CFDCA3-71A5-DD4D-9D0E-D63068092BC8}">
   <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,31 +1234,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1556,7 +1609,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <f>P8/D7</f>
         <v>-0.10054184226369657</v>
       </c>
@@ -1571,4 +1624,369 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02857098-9EF4-7A43-8BB2-8228CE41206A}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4">
+        <v>127</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>153</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>459</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>314</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>284</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>45</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>162</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>162</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>140</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>36</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <v>44</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13">
+        <v>64</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>22</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15">
+        <v>85</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16">
+        <v>81</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <f>SUM(B3:B17)</f>
+        <v>1588</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" ref="C18:G18" si="0">SUM(C3:C17)</f>
+        <v>51</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>836</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <f>E18-B18</f>
+        <v>-752</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E20" s="4">
+        <f>E19/B18</f>
+        <v>-0.47355163727959698</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>